<commit_message>
Updates to eps-eu commit #21ff0b1
</commit_message>
<xml_diff>
--- a/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
+++ b/InputData/elec/BPSpUGBCD/BAU Subsidy per Unit Grid Battery Capacity Deployed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BPSpUGBCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40724972-2873-4441-97DA-52FF5D7F6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1640CF-E3B7-443F-9523-22E8743CB9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,7 +979,7 @@
   <dimension ref="A1:AJ534"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="V75" sqref="V75:Y75"/>
+      <selection activeCell="U75" sqref="U75:X75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4614,13 +4614,13 @@
         <v>1</v>
       </c>
       <c r="V75" s="37">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="W75" s="37">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="X75" s="37">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y75" s="37">
         <v>0</v>
@@ -5271,15 +5271,15 @@
       </c>
       <c r="U88" s="38">
         <f t="shared" si="5"/>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="V88" s="38">
         <f t="shared" si="5"/>
-        <v>0.31218750000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="W88" s="31">
         <f t="shared" si="5"/>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="X88" s="31">
         <f t="shared" si="5"/>
@@ -22471,15 +22471,15 @@
       </c>
       <c r="W2" s="2">
         <f>'Inflation Reduction Act'!U88</f>
-        <v>0.41625000000000001</v>
+        <v>0.31218750000000001</v>
       </c>
       <c r="X2" s="2">
         <f>'Inflation Reduction Act'!V88</f>
-        <v>0.31218750000000001</v>
+        <v>0.208125</v>
       </c>
       <c r="Y2" s="2">
         <f>'Inflation Reduction Act'!W88</f>
-        <v>0.208125</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="2">
         <f>'Inflation Reduction Act'!X88</f>

</xml_diff>